<commit_message>
add first class soul
</commit_message>
<xml_diff>
--- a/enemy.xlsx
+++ b/enemy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,6 +140,12 @@
   <si>
     <t>weaponlskilllevel</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENEMY_NAME_3</t>
+  </si>
+  <si>
+    <t>ENEMY_DESC_3</t>
   </si>
 </sst>
 </file>
@@ -483,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -595,16 +601,16 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>2000</v>
@@ -619,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -678,22 +684,22 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>2400</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -702,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>1001</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -747,6 +753,89 @@
         <v>1</v>
       </c>
       <c r="AA3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>2400</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>5000</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>3</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
skill energy cost change to 1
</commit_message>
<xml_diff>
--- a/enemy.xlsx
+++ b/enemy.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="360" windowWidth="17960" windowHeight="11340"/>
+    <workbookView xWindow="720" yWindow="360" windowWidth="17955" windowHeight="11340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -156,8 +156,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,10 +202,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -493,26 +498,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="Y7" sqref="Y7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="3" width="14.5" customWidth="1"/>
     <col min="9" max="11" width="15" customWidth="1"/>
-    <col min="14" max="14" width="10.1640625" customWidth="1"/>
+    <col min="14" max="14" width="10.125" customWidth="1"/>
     <col min="15" max="15" width="18" customWidth="1"/>
-    <col min="17" max="21" width="13.1640625" customWidth="1"/>
-    <col min="23" max="24" width="10.6640625" customWidth="1"/>
-    <col min="25" max="25" width="10.1640625" customWidth="1"/>
+    <col min="17" max="21" width="13.125" customWidth="1"/>
+    <col min="23" max="24" width="10.625" customWidth="1"/>
+    <col min="25" max="25" width="10.125" customWidth="1"/>
     <col min="26" max="26" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -595,7 +600,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -606,7 +611,7 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -678,7 +683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -761,7 +766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -856,12 +861,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -874,12 +879,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>